<commit_message>
change logo game by login logout (JHipster sample)
</commit_message>
<xml_diff>
--- a/src/main/resources/archetype-resources/src/test/resources/data/in/__targetApplicationName__.xlsx
+++ b/src/main/resources/archetype-resources/src/test/resources/data/in/__targetApplicationName__.xlsx
@@ -17,66 +17,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="3">
   <si>
     <t>Résultat</t>
   </si>
   <si>
-    <t>Peter</t>
+    <t>user</t>
   </si>
   <si>
-    <t>player</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>Wendy</t>
-  </si>
-  <si>
-    <t>amazon</t>
-  </si>
-  <si>
-    <t>ebay</t>
-  </si>
-  <si>
-    <t>michelin</t>
-  </si>
-  <si>
-    <t>napster</t>
-  </si>
-  <si>
-    <t>pringles</t>
-  </si>
-  <si>
-    <t>reebook</t>
-  </si>
-  <si>
-    <t>twitter</t>
-  </si>
-  <si>
-    <t>youtube</t>
-  </si>
-  <si>
-    <t>Mr Bean</t>
-  </si>
-  <si>
-    <t>fake</t>
-  </si>
-  <si>
-    <t>score</t>
-  </si>
-  <si>
-    <t>burger king</t>
-  </si>
-  <si>
-    <t>hello kitty</t>
-  </si>
-  <si>
-    <t>red bull</t>
-  </si>
-  <si>
-    <t>citroën</t>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -180,7 +129,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -504,299 +460,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -854,19 +707,19 @@
       <c r="A50" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>COUNTIFS($A:$A,$A6,$D:$D, "Échec :*") &gt; 0</formula>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>COUNTIFS($A:$A,$A6,$C:$C, "Échec :*") &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>COUNTIFS($A:$A,$A16,$D:$D, "Échec :*") &gt; 0</formula>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>COUNTIFS($A:$A,$A16,$C:$C, "Échec :*") &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D24">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>COUNTIFS($A:$A,$A2,$D:$D, "Échec :*") &gt; 0</formula>
+  <conditionalFormatting sqref="A2:C24">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>COUNTIFS($A:$A,$A2,$C:$C, "Échec :*") &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>